<commit_message>
synchro + some design
</commit_message>
<xml_diff>
--- a/Assets/csv/billiejean.xlsx
+++ b/Assets/csv/billiejean.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\UnityProjectMusicalInstrument\Assets\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohamed khrouf\Desktop\unity\UnityProjectMusicalInstrument\Assets\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A223F4-F42A-4FAB-8919-EED7B6D62CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,16 +361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ER1" workbookViewId="0">
-      <selection activeCell="FE2" sqref="FE2:FX2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:237" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -396,7 +395,7 @@
         <v>1.2931034482758599</v>
       </c>
       <c r="G1">
-        <f t="shared" si="0"/>
+        <f>F1+0.517241379310344/2</f>
         <v>1.5517241379310318</v>
       </c>
       <c r="H1">
@@ -1320,7 +1319,7 @@
         <v>61.034482758620804</v>
       </c>
     </row>
-    <row r="2" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:237" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:237" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2974,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:237" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:237" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>